<commit_message>
Used sieve of erasthothenes
</commit_message>
<xml_diff>
--- a/PrimeSumCalc/Results.xlsx
+++ b/PrimeSumCalc/Results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wutwaw-my.sharepoint.com/personal/01169583_pw_edu_pl/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkuzm\Desktop\Parallel-and-Distributed-Programming\PrimeSumCalc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F27BEDA3-F4E6-4069-A9B1-04AB6D26A404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB1C551-C923-4F0B-8BD2-42680B3E04F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6257BE5F-9BAA-4DAD-9CBD-6CA907FF725B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Number Of Processes</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Number Of Prime Numbers</t>
-  </si>
-  <si>
-    <t>The time is almost the same up to 10 millions (10000000) prime numbers</t>
   </si>
 </sst>
 </file>
@@ -170,8 +167,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -213,66 +209,60 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$A$2:$A$9</c:f>
+              <c:f>Arkusz1!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$B$2:$B$9</c:f>
+              <c:f>Arkusz1!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4.6875E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>1.234375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.140625</c:v>
+                  <c:v>12.859375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78125</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.328125</c:v>
+                  <c:v>63.828125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.859375</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>14.46875</c:v>
+                  <c:v>134.0625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,7 +351,8 @@
         <c:axId val="1712305424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="14"/>
+          <c:max val="150"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -627,32 +618,35 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Arkusz1!$H$2:$H$9</c:f>
+              <c:f>Arkusz1!$H$2:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>20000</c:v>
                 </c:pt>
               </c:numCache>
@@ -660,10 +654,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Arkusz1!$I$2:$I$9</c:f>
+              <c:f>Arkusz1!$I$2:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -671,22 +665,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.125</c:v>
+                  <c:v>0.109375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.796875</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4375</c:v>
+                  <c:v>1.859375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.890625</c:v>
+                  <c:v>6.640625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.578125</c:v>
+                  <c:v>18.109375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60.375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2391,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060C4624-ED47-49F9-A3CA-F17BB01BECE1}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,7 +2402,7 @@
     <col min="10" max="10" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2424,168 +2421,176 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="C2">
-        <v>100000</v>
+        <v>84000000</v>
       </c>
       <c r="H2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>750000</v>
+        <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4.6875E-2</v>
       </c>
       <c r="C3">
-        <v>100000</v>
+        <v>84000000</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>750000</v>
+        <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0.125</v>
+      </c>
+      <c r="C4">
+        <v>84000000</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>1.234375</v>
+      </c>
+      <c r="C5">
+        <v>84000000</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>0.109375</v>
+      </c>
+      <c r="J5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>1000</v>
       </c>
-      <c r="B4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C4">
-        <v>100000</v>
-      </c>
-      <c r="H4">
+      <c r="B6">
+        <v>12.859375</v>
+      </c>
+      <c r="C6">
+        <v>84000000</v>
+      </c>
+      <c r="H6">
         <v>1000</v>
       </c>
-      <c r="I4">
-        <v>3.125E-2</v>
-      </c>
-      <c r="J4">
-        <v>750000</v>
+      <c r="I6">
+        <v>0.8125</v>
+      </c>
+      <c r="J6">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2000</v>
       </c>
-      <c r="B5">
-        <v>0.140625</v>
-      </c>
-      <c r="C5">
-        <v>100000</v>
-      </c>
-      <c r="H5">
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>84000000</v>
+      </c>
+      <c r="H7">
         <v>2000</v>
       </c>
-      <c r="I5">
-        <v>0.125</v>
-      </c>
-      <c r="J5">
-        <v>750000</v>
+      <c r="I7">
+        <v>1.859375</v>
+      </c>
+      <c r="J7">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>5000</v>
       </c>
-      <c r="B6">
-        <v>0.78125</v>
-      </c>
-      <c r="C6">
-        <v>100000</v>
-      </c>
-      <c r="H6">
+      <c r="B8">
+        <v>63.828125</v>
+      </c>
+      <c r="C8">
+        <v>84000000</v>
+      </c>
+      <c r="H8">
         <v>5000</v>
       </c>
-      <c r="I6">
-        <v>0.796875</v>
-      </c>
-      <c r="J6">
-        <v>750000</v>
+      <c r="I8">
+        <v>6.640625</v>
+      </c>
+      <c r="J8">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>10000</v>
       </c>
-      <c r="B7">
-        <v>3.328125</v>
-      </c>
-      <c r="C7">
-        <v>100000</v>
-      </c>
-      <c r="H7">
+      <c r="B9">
+        <v>134.0625</v>
+      </c>
+      <c r="C9">
+        <v>84000000</v>
+      </c>
+      <c r="H9">
         <v>10000</v>
       </c>
-      <c r="I7">
-        <v>3.4375</v>
-      </c>
-      <c r="J7">
-        <v>750000</v>
+      <c r="I9">
+        <v>18.109375</v>
+      </c>
+      <c r="J9">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>15000</v>
-      </c>
-      <c r="B8">
-        <v>7.859375</v>
-      </c>
-      <c r="C8">
-        <v>100000</v>
-      </c>
-      <c r="H8">
-        <v>15000</v>
-      </c>
-      <c r="I8">
-        <v>7.890625</v>
-      </c>
-      <c r="J8">
-        <v>750000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10">
         <v>20000</v>
       </c>
-      <c r="B9">
-        <v>14.46875</v>
-      </c>
-      <c r="C9">
-        <v>100000</v>
-      </c>
-      <c r="H9">
-        <v>20000</v>
-      </c>
-      <c r="I9">
-        <v>14.578125</v>
-      </c>
-      <c r="J9">
-        <v>750000</v>
+      <c r="I10">
+        <v>60.375</v>
+      </c>
+      <c r="J10">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>